<commit_message>
dasde - excel formula conversion.
</commit_message>
<xml_diff>
--- a/dasde 15/red.xlsx
+++ b/dasde 15/red.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NiTe\Desktop\red\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asadtariq/Downloads/Python_work/Python_work/dasde 15/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A261A3F7-DA8E-47FF-9834-11F43020500F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E598B85B-4BFC-7B4E-999C-8834F51A8289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="1440" windowWidth="21600" windowHeight="11295" xr2:uid="{23C80F8A-58F4-4786-9AE1-BE0D42BDC793}"/>
+    <workbookView xWindow="2380" yWindow="1440" windowWidth="21600" windowHeight="11300" xr2:uid="{23C80F8A-58F4-4786-9AE1-BE0D42BDC793}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Condition</t>
   </si>
@@ -431,21 +433,21 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -496,7 +498,7 @@
       </c>
       <c r="E2">
         <f>+IF(A2="n","",COUNTIF(D3:$D10000,$D2))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
         <f>B2+1</f>
@@ -508,7 +510,7 @@
       </c>
       <c r="H2">
         <f>+IF(A2="n","",COUNTIF(D3:$D10000,$G2))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1">
         <f>B2+2</f>
@@ -524,7 +526,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -567,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -610,7 +612,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -626,7 +628,7 @@
       </c>
       <c r="E5">
         <f>+IF(A5="n","",COUNTIF(D6:$D10003,$D5))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1">
         <f>B5+1</f>
@@ -638,7 +640,7 @@
       </c>
       <c r="H5">
         <f>+IF(A5="n","",COUNTIF(D6:$D10003,$G5))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" s="1">
         <f>B5+2</f>
@@ -653,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -669,7 +671,7 @@
       </c>
       <c r="E6">
         <f>+IF(A6="n","",COUNTIF(D7:$D10004,$D6))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6:F8" si="5">B6+1</f>
@@ -696,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -712,7 +714,7 @@
       </c>
       <c r="E7">
         <f>+IF(A7="n","",COUNTIF(D8:$D10005,$D7))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="5"/>
@@ -739,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -778,375 +780,488 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44593</v>
+      </c>
+      <c r="C9">
+        <v>1234567</v>
+      </c>
       <c r="D9" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE(B9,C9)</f>
+        <v>445931234567</v>
+      </c>
+      <c r="E9">
+        <f>+IF(A9="n","",COUNTIF(D10:$D10007,$D9))</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <f>B9+1</f>
+        <v>44594</v>
+      </c>
+      <c r="G9" t="str">
+        <f>CONCATENATE(F9,C9)</f>
+        <v>445941234567</v>
+      </c>
+      <c r="H9">
+        <f>+IF(A9="n","",COUNTIF(D10:$D10007,$G9))</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <f>B9+2</f>
+        <v>44595</v>
+      </c>
+      <c r="J9" t="str">
+        <f>CONCATENATE(I9,C9)</f>
+        <v>445951234567</v>
+      </c>
+      <c r="K9">
+        <f>+IF(A9="n","",COUNTIF(D10:$D10007,$J9))</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44593</v>
+      </c>
+      <c r="C10">
+        <v>1234567</v>
+      </c>
       <c r="D10" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE(B10,C10)</f>
+        <v>445931234567</v>
+      </c>
+      <c r="E10">
+        <f>+IF(A10="n","",COUNTIF(D11:$D10008,$D10))</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <f>B10+1</f>
+        <v>44594</v>
+      </c>
+      <c r="G10" t="str">
+        <f>CONCATENATE(F10,C10)</f>
+        <v>445941234567</v>
+      </c>
+      <c r="H10">
+        <f>+IF(A10="n","",COUNTIF(D11:$D10008,$G10))</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <f>B10+2</f>
+        <v>44595</v>
+      </c>
+      <c r="J10" t="str">
+        <f>CONCATENATE(I10,C10)</f>
+        <v>445951234567</v>
+      </c>
+      <c r="K10">
+        <f>+IF(A10="n","",COUNTIF(D11:$D10008,$J10))</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44594</v>
+      </c>
+      <c r="C11">
+        <v>1234567</v>
+      </c>
       <c r="D11" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE(B11,C11)</f>
+        <v>445941234567</v>
+      </c>
+      <c r="E11">
+        <f>+IF(A11="n","",COUNTIF(D12:$D10009,$D11))</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" ref="F11" si="7">B11+1</f>
+        <v>44595</v>
+      </c>
+      <c r="G11" t="str">
+        <f>CONCATENATE(F11,C12)</f>
+        <v>44595</v>
+      </c>
+      <c r="H11">
+        <f>+IF(A11="n","",COUNTIF(D12:$D10009,$G11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>B11+2</f>
+        <v>44596</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ref="J11" si="8">CONCATENATE(I11,C11)</f>
+        <v>445961234567</v>
+      </c>
+      <c r="K11">
+        <f>+IF(A11="n","",COUNTIF(D12:$D10009,$J11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D32" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D42" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D43" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D48" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D50" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D51" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D52" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D53" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D54" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D55" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D56" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D57" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D58" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D59" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D60" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D61" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D62" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D63" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D64" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D66" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D67" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D68" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D69" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D70" t="str">
-        <f t="shared" ref="D70" si="7">CONCATENATE(B70,C70)</f>
+        <f t="shared" ref="D70" si="9">CONCATENATE(B70,C70)</f>
         <v/>
       </c>
     </row>

</xml_diff>